<commit_message>
mapas antes de clusterizacion
</commit_message>
<xml_diff>
--- a/data/poblacionParroquias.xlsx
+++ b/data/poblacionParroquias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreidavid.flores\Downloads\Work\Parroquias Datos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5C8A61-0391-4D0B-BFF4-0DB058C7E70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2450CA-6828-4036-AB6F-C309864D3BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{D415D4B0-127F-48D1-B64E-658D162E9589}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>Rumiñahui</t>
   </si>
   <si>
-    <t>Los chillos</t>
-  </si>
-  <si>
     <t>Distrito Metropolitano de Quito</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>Fajardo</t>
+  </si>
+  <si>
+    <t>Cotogchoa</t>
   </si>
 </sst>
 </file>
@@ -316,10 +316,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,15 +655,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA06E173-C984-4F10-8991-91694CAC44A4}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -679,7 +681,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -690,7 +692,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>1285291</v>
@@ -707,7 +709,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3">
         <v>1285291</v>
@@ -724,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>1285291</v>
@@ -741,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5">
         <v>1285291</v>
@@ -758,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>1285291</v>
@@ -775,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="D7">
         <v>1285291</v>
@@ -789,10 +791,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
       </c>
       <c r="D8">
         <v>250877</v>
@@ -806,10 +808,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>127815</v>
@@ -823,10 +825,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>115961</v>
@@ -840,10 +842,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <v>108989</v>
@@ -857,10 +859,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>100374</v>
@@ -874,10 +876,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13">
         <v>93005</v>
@@ -891,10 +893,10 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <v>79109</v>
@@ -908,10 +910,10 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15">
         <v>74959</v>
@@ -925,10 +927,10 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16">
         <v>72489</v>
@@ -942,10 +944,10 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17">
         <v>68773</v>
@@ -959,10 +961,10 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18">
         <v>68701</v>
@@ -976,10 +978,10 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19">
         <v>67241</v>
@@ -993,10 +995,10 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20">
         <v>64226</v>
@@ -1010,10 +1012,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21">
         <v>63009</v>
@@ -1027,10 +1029,10 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22">
         <v>62095</v>
@@ -1044,10 +1046,10 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23">
         <v>61367</v>
@@ -1061,10 +1063,10 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24">
         <v>58715</v>
@@ -1078,10 +1080,10 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25">
         <v>56184</v>
@@ -1095,10 +1097,10 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26">
         <v>54478</v>
@@ -1112,10 +1114,10 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D27">
         <v>53253</v>
@@ -1129,10 +1131,10 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28">
         <v>50500</v>
@@ -1146,10 +1148,10 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D29">
         <v>49984</v>
@@ -1163,10 +1165,10 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30">
         <v>49573</v>
@@ -1180,10 +1182,10 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31">
         <v>47695</v>
@@ -1197,10 +1199,10 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D32">
         <v>47679</v>
@@ -1214,10 +1216,10 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D33">
         <v>46244</v>
@@ -1231,10 +1233,10 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34">
         <v>43235</v>
@@ -1248,10 +1250,10 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35">
         <v>41819</v>
@@ -1265,10 +1267,10 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36">
         <v>37491</v>
@@ -1282,10 +1284,10 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D37">
         <v>36883</v>
@@ -1299,10 +1301,10 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D38">
         <v>34655</v>
@@ -1316,10 +1318,10 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39">
         <v>34380</v>
@@ -1333,10 +1335,10 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40">
         <v>32652</v>
@@ -1350,10 +1352,10 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D41">
         <v>32610</v>
@@ -1367,10 +1369,10 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D42">
         <v>30245</v>
@@ -1384,10 +1386,10 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D43">
         <v>29509</v>
@@ -1401,10 +1403,10 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44">
         <v>28579</v>
@@ -1418,10 +1420,10 @@
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45">
         <v>27092</v>
@@ -1435,10 +1437,10 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46">
         <v>26564</v>
@@ -1452,10 +1454,10 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47">
         <v>23240</v>
@@ -1469,10 +1471,10 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48">
         <v>23224</v>
@@ -1486,10 +1488,10 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49">
         <v>23202</v>
@@ -1503,10 +1505,10 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50">
         <v>22065</v>
@@ -1520,10 +1522,10 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D51">
         <v>20584</v>
@@ -1537,10 +1539,10 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52">
         <v>18485</v>
@@ -1554,10 +1556,10 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53">
         <v>17780</v>
@@ -1571,10 +1573,10 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D54">
         <v>15113</v>
@@ -1588,10 +1590,10 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55">
         <v>15072</v>
@@ -1605,10 +1607,10 @@
         <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D56">
         <v>11492</v>
@@ -1622,10 +1624,10 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D57">
         <v>11438</v>
@@ -1639,10 +1641,10 @@
         <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D58">
         <v>6160</v>
@@ -1656,10 +1658,10 @@
         <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D59">
         <v>5589</v>
@@ -1673,10 +1675,10 @@
         <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D60">
         <v>5155</v>
@@ -1690,10 +1692,10 @@
         <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D61">
         <v>4964</v>
@@ -1707,10 +1709,10 @@
         <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D62">
         <v>4336</v>
@@ -1724,10 +1726,10 @@
         <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D63">
         <v>3898</v>
@@ -1741,10 +1743,10 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D64">
         <v>3851</v>
@@ -1758,10 +1760,10 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D65">
         <v>2959</v>
@@ -1775,10 +1777,10 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D66">
         <v>2938</v>
@@ -1792,10 +1794,10 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D67">
         <v>2776</v>
@@ -1809,10 +1811,10 @@
         <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D68">
         <v>1959</v>
@@ -1826,10 +1828,10 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D69">
         <v>1704</v>
@@ -1843,10 +1845,10 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D70">
         <v>1446</v>
@@ -1860,10 +1862,10 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D71">
         <v>704</v>
@@ -1877,10 +1879,10 @@
         <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D72">
         <v>579</v>

</xml_diff>